<commit_message>
ci: pretas may 2021 - fix some forms errors
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_2_participant_202105.xlsx
+++ b/LF/PreTAS/Ivory Coast/May 2021/ci_lf_pretas_2_participant_202105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\May 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ACB4DD-9B0B-4882-889D-ABAE098C753F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69739BE-FBCC-44D1-8530-09912F20F021}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -335,27 +335,9 @@
     <t>p_num</t>
   </si>
   <si>
-    <t>Entrer le numéro d'ordre</t>
-  </si>
-  <si>
     <t>Enter the order number</t>
   </si>
   <si>
-    <t>Must be between 1 and 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doit être compris entre 1 et 300 </t>
-  </si>
-  <si>
-    <t>. &gt; 0 and . &lt;= 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La valeur doit être compris entre 1 et 300 </t>
-  </si>
-  <si>
-    <t>The value must be between 1 and 300</t>
-  </si>
-  <si>
     <t>if(${p_site_name} = 'Autre', concat(${p_site_id2}, '-' ,${p_num}), concat(${p_site_id}, '-' ,${p_num}))</t>
   </si>
   <si>
@@ -365,10 +347,28 @@
     <t>Code d'identification du répondant (Veuillez recopier ce code tel qu'il est quelque part entre autre sur les test de diagnostique)</t>
   </si>
   <si>
-    <t>(May 2021) 2. Côte d'Ivoire -  Pre TAS FL Formulaire Participants V3</t>
-  </si>
-  <si>
-    <t>ci_lf_pretas_2_participant_202105_v3</t>
+    <t>ci_lf_pretas_2_participant_202105_v4</t>
+  </si>
+  <si>
+    <t>(May 2021) 2. Côte d'Ivoire -  Pre TAS FL Formulaire Participants V4</t>
+  </si>
+  <si>
+    <t>Must be between 1 and 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doit être compris entre 1 et 500 </t>
+  </si>
+  <si>
+    <t>. &gt; 0 and . &lt;= 500</t>
+  </si>
+  <si>
+    <t>The value must be between 1 and 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La valeur doit être compris entre 1 et 500 </t>
+  </si>
+  <si>
+    <t>Répeter le numéro d'ordre</t>
   </si>
 </sst>
 </file>
@@ -830,11 +830,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="4" t="s">
@@ -1137,26 +1137,26 @@
         <v>100</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>70</v>
@@ -1282,14 +1282,14 @@
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F14" s="11"/>
       <c r="K14" s="1" t="s">
         <v>70</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>73</v>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C2">
         <v>20210511</v>

</xml_diff>